<commit_message>
nueva version de datos de horarios del metro, eliminacion de plaza de armas L3
</commit_message>
<xml_diff>
--- a/src/horarios/HorariosMetro.xlsx
+++ b/src/horarios/HorariosMetro.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\GTFSProcessing\horarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\GTFSProcessing\src\horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21900" windowHeight="10200" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21900" windowHeight="10200" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="L1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5993" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6035" uniqueCount="281">
   <si>
     <t>Codigo</t>
   </si>
@@ -862,6 +862,24 @@
   <si>
     <t>Agustin 2</t>
   </si>
+  <si>
+    <t>Matta</t>
+  </si>
+  <si>
+    <t>Irarrazabal</t>
+  </si>
+  <si>
+    <t>Monseñor Eyzaguirre</t>
+  </si>
+  <si>
+    <t>Chile España</t>
+  </si>
+  <si>
+    <t>Pdte. Pedro Aguirre Cerda</t>
+  </si>
+  <si>
+    <t>PG</t>
+  </si>
 </sst>
 </file>
 
@@ -882,7 +900,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -949,6 +967,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFECE4E1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCBAB3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -977,7 +1007,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1031,6 +1061,15 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="20" fontId="1" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1313,8 +1352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P82"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection sqref="A1:P82"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5194,7 +5233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+    <sheetView topLeftCell="A87" workbookViewId="0">
       <selection activeCell="Q93" sqref="Q93"/>
     </sheetView>
   </sheetViews>
@@ -15199,8 +15238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P91"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:P91"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19780,7 +19819,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:P31"/>
+      <selection activeCell="A2" sqref="A2:O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19935,13 +19974,13 @@
     </row>
     <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>202</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>232</v>
+        <v>280</v>
       </c>
       <c r="C4" t="s">
-        <v>231</v>
+        <v>279</v>
       </c>
       <c r="D4" t="s">
         <v>228</v>
@@ -20345,13 +20384,13 @@
     </row>
     <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>202</v>
+        <v>103</v>
       </c>
       <c r="B14" t="s">
-        <v>232</v>
+        <v>280</v>
       </c>
       <c r="C14" t="s">
-        <v>231</v>
+        <v>279</v>
       </c>
       <c r="D14" t="s">
         <v>228</v>
@@ -20755,13 +20794,13 @@
     </row>
     <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>202</v>
+        <v>103</v>
       </c>
       <c r="B24" t="s">
-        <v>232</v>
+        <v>280</v>
       </c>
       <c r="C24" t="s">
-        <v>231</v>
+        <v>279</v>
       </c>
       <c r="D24" t="s">
         <v>228</v>
@@ -21090,8 +21129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:P55"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:O55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21113,7 +21152,7 @@
     <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -21163,7 +21202,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>108</v>
       </c>
@@ -21179,14 +21218,32 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
+      <c r="F2" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I2" s="19">
+        <v>0.98263888888888884</v>
+      </c>
       <c r="J2" t="s">
         <v>242</v>
       </c>
+      <c r="K2" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="M2" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N2" s="19">
+        <v>0.24374999999999999</v>
+      </c>
+      <c r="O2" s="19">
+        <v>0.96180555555555547</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>109</v>
       </c>
@@ -21202,14 +21259,32 @@
       <c r="E3" t="s">
         <v>9</v>
       </c>
+      <c r="F3" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I3" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="J3" t="s">
         <v>242</v>
       </c>
+      <c r="K3" s="19">
+        <v>0.24374999999999999</v>
+      </c>
+      <c r="L3" s="19">
+        <v>0.98402777777777783</v>
+      </c>
       <c r="M3" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N3" s="19">
+        <v>0.24444444444444446</v>
+      </c>
+      <c r="O3" s="19">
+        <v>0.96319444444444446</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>110</v>
       </c>
@@ -21225,14 +21300,32 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
+      <c r="F4" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I4" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="J4" t="s">
         <v>242</v>
       </c>
+      <c r="K4" s="19">
+        <v>0.24513888888888888</v>
+      </c>
+      <c r="L4" s="19">
+        <v>0.98263888888888884</v>
+      </c>
       <c r="M4" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N4" s="19">
+        <v>0.24652777777777779</v>
+      </c>
+      <c r="O4" s="19">
+        <v>0.96527777777777779</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>111</v>
       </c>
@@ -21248,14 +21341,32 @@
       <c r="E5" t="s">
         <v>9</v>
       </c>
+      <c r="F5" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I5" s="19">
+        <v>0.97569444444444453</v>
+      </c>
       <c r="J5" t="s">
         <v>242</v>
       </c>
+      <c r="K5" s="19">
+        <v>0.24444444444444446</v>
+      </c>
+      <c r="L5" s="19">
+        <v>0.98055555555555562</v>
+      </c>
       <c r="M5" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N5" s="19">
+        <v>0.24791666666666667</v>
+      </c>
+      <c r="O5" s="19">
+        <v>0.96666666666666667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>112</v>
       </c>
@@ -21271,14 +21382,32 @@
       <c r="E6" t="s">
         <v>9</v>
       </c>
+      <c r="F6" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I6" s="19">
+        <v>0.97569444444444453</v>
+      </c>
       <c r="J6" t="s">
         <v>242</v>
       </c>
+      <c r="K6" s="19">
+        <v>0.24583333333333335</v>
+      </c>
+      <c r="L6" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="M6" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N6" s="19">
+        <v>0.24374999999999999</v>
+      </c>
+      <c r="O6" s="19">
+        <v>0.96805555555555556</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>113</v>
       </c>
@@ -21294,14 +21423,32 @@
       <c r="E7" t="s">
         <v>9</v>
       </c>
+      <c r="F7" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I7" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="J7" t="s">
         <v>242</v>
       </c>
+      <c r="K7" s="19">
+        <v>0.24444444444444446</v>
+      </c>
+      <c r="L7" s="19">
+        <v>0.97777777777777775</v>
+      </c>
       <c r="M7" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N7" s="19">
+        <v>0.24444444444444446</v>
+      </c>
+      <c r="O7" s="19">
+        <v>0.96944444444444444</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>12</v>
       </c>
@@ -21317,14 +21464,32 @@
       <c r="E8" t="s">
         <v>9</v>
       </c>
+      <c r="F8" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I8" s="19">
+        <v>0.97361111111111109</v>
+      </c>
       <c r="J8" t="s">
         <v>242</v>
       </c>
+      <c r="K8" s="19">
+        <v>0.25208333333333333</v>
+      </c>
+      <c r="L8" s="19">
+        <v>0.97638888888888886</v>
+      </c>
       <c r="M8" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N8" s="19">
+        <v>0.25138888888888888</v>
+      </c>
+      <c r="O8" s="19">
+        <v>0.97083333333333333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>114</v>
       </c>
@@ -21340,14 +21505,32 @@
       <c r="E9" t="s">
         <v>9</v>
       </c>
+      <c r="F9" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I9" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="J9" t="s">
         <v>242</v>
       </c>
+      <c r="K9" s="19">
+        <v>0.24444444444444446</v>
+      </c>
+      <c r="L9" s="19">
+        <v>0.97499999999999998</v>
+      </c>
       <c r="M9" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N9" s="19">
+        <v>0.24444444444444446</v>
+      </c>
+      <c r="O9" s="19">
+        <v>0.97222222222222221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>15</v>
       </c>
@@ -21363,14 +21546,32 @@
       <c r="E10" t="s">
         <v>9</v>
       </c>
+      <c r="F10" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I10" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="J10" t="s">
         <v>242</v>
       </c>
+      <c r="K10" s="19">
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="L10" s="19">
+        <v>0.97361111111111109</v>
+      </c>
       <c r="M10" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N10" s="19">
+        <v>0.2388888888888889</v>
+      </c>
+      <c r="O10" s="19">
+        <v>0.97361111111111109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>115</v>
       </c>
@@ -21386,14 +21587,32 @@
       <c r="E11" t="s">
         <v>9</v>
       </c>
+      <c r="F11" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I11" s="19">
+        <v>0.96875</v>
+      </c>
       <c r="J11" t="s">
         <v>242</v>
       </c>
+      <c r="K11" s="19">
+        <v>0.24583333333333335</v>
+      </c>
+      <c r="L11" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="M11" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N11" s="19">
+        <v>0.24374999999999999</v>
+      </c>
+      <c r="O11" s="19">
+        <v>0.97430555555555554</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>116</v>
       </c>
@@ -21409,14 +21628,32 @@
       <c r="E12" t="s">
         <v>9</v>
       </c>
+      <c r="F12" s="21">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I12" s="21">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="J12" t="s">
         <v>242</v>
       </c>
+      <c r="K12" s="21">
+        <v>0.24374999999999999</v>
+      </c>
+      <c r="L12" s="21">
+        <v>0.97152777777777777</v>
+      </c>
       <c r="M12" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N12" s="21">
+        <v>0.24583333333333335</v>
+      </c>
+      <c r="O12" s="21">
+        <v>0.97638888888888886</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>35</v>
       </c>
@@ -21432,14 +21669,32 @@
       <c r="E13" t="s">
         <v>9</v>
       </c>
+      <c r="F13" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I13" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="J13" t="s">
         <v>242</v>
       </c>
+      <c r="K13" s="19">
+        <v>0.24583333333333335</v>
+      </c>
+      <c r="L13" s="19">
+        <v>0.96944444444444444</v>
+      </c>
       <c r="M13" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N13" s="19">
+        <v>0.24374999999999999</v>
+      </c>
+      <c r="O13" s="19">
+        <v>0.97777777777777775</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>117</v>
       </c>
@@ -21455,14 +21710,32 @@
       <c r="E14" t="s">
         <v>9</v>
       </c>
+      <c r="F14" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I14" s="19">
+        <v>0.97569444444444453</v>
+      </c>
       <c r="J14" t="s">
         <v>242</v>
       </c>
+      <c r="K14" s="19">
+        <v>0.24444444444444446</v>
+      </c>
+      <c r="L14" s="19">
+        <v>0.96805555555555556</v>
+      </c>
       <c r="M14" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N14" s="19">
+        <v>0.24444444444444446</v>
+      </c>
+      <c r="O14" s="19">
+        <v>0.97916666666666663</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>106</v>
       </c>
@@ -21478,14 +21751,32 @@
       <c r="E15" t="s">
         <v>9</v>
       </c>
+      <c r="F15" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I15" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="J15" t="s">
         <v>242</v>
       </c>
+      <c r="K15" s="19">
+        <v>0.23819444444444446</v>
+      </c>
+      <c r="L15" s="19">
+        <v>0.96666666666666667</v>
+      </c>
       <c r="M15" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N15" s="19">
+        <v>0.23819444444444446</v>
+      </c>
+      <c r="O15" s="19">
+        <v>0.97986111111111107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>118</v>
       </c>
@@ -21501,14 +21792,32 @@
       <c r="E16" t="s">
         <v>9</v>
       </c>
+      <c r="F16" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I16" s="19">
+        <v>0.97569444444444453</v>
+      </c>
       <c r="J16" t="s">
         <v>242</v>
       </c>
+      <c r="K16" s="19">
+        <v>0.24444444444444446</v>
+      </c>
+      <c r="L16" s="19">
+        <v>0.96597222222222223</v>
+      </c>
       <c r="M16" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="19">
+        <v>0.24652777777777779</v>
+      </c>
+      <c r="O16" s="19">
+        <v>0.98125000000000007</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>119</v>
       </c>
@@ -21524,14 +21833,32 @@
       <c r="E17" t="s">
         <v>9</v>
       </c>
+      <c r="F17" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I17" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="J17" t="s">
         <v>242</v>
       </c>
+      <c r="K17" s="19">
+        <v>0.24583333333333335</v>
+      </c>
+      <c r="L17" s="19">
+        <v>0.96458333333333324</v>
+      </c>
       <c r="M17" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="19">
+        <v>0.24791666666666667</v>
+      </c>
+      <c r="O17" s="19">
+        <v>0.98263888888888884</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>24</v>
       </c>
@@ -21547,14 +21874,32 @@
       <c r="E18" t="s">
         <v>9</v>
       </c>
+      <c r="F18" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I18" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="J18" t="s">
         <v>242</v>
       </c>
+      <c r="K18" s="19">
+        <v>0.24444444444444446</v>
+      </c>
+      <c r="L18" s="19">
+        <v>0.96319444444444446</v>
+      </c>
       <c r="M18" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="19">
+        <v>0.24930555555555556</v>
+      </c>
+      <c r="O18" s="19">
+        <v>0.98402777777777783</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>120</v>
       </c>
@@ -21570,14 +21915,32 @@
       <c r="E19" t="s">
         <v>9</v>
       </c>
+      <c r="F19" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I19" s="19">
+        <v>0.98263888888888884</v>
+      </c>
       <c r="J19" t="s">
         <v>242</v>
       </c>
+      <c r="K19" s="19">
+        <v>0.24583333333333335</v>
+      </c>
+      <c r="L19" s="19">
+        <v>0.96180555555555547</v>
+      </c>
       <c r="M19" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="O19" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>108</v>
       </c>
@@ -21593,14 +21956,32 @@
       <c r="E20" t="s">
         <v>72</v>
       </c>
+      <c r="F20" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I20" s="19">
+        <v>0.98263888888888884</v>
+      </c>
       <c r="J20" t="s">
         <v>242</v>
       </c>
+      <c r="K20" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="M20" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20" s="19">
+        <v>0.27152777777777776</v>
+      </c>
+      <c r="O20" s="19">
+        <v>0.96180555555555547</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>109</v>
       </c>
@@ -21616,14 +21997,32 @@
       <c r="E21" t="s">
         <v>72</v>
       </c>
+      <c r="F21" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I21" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="J21" t="s">
         <v>242</v>
       </c>
+      <c r="K21" s="19">
+        <v>0.27152777777777776</v>
+      </c>
+      <c r="L21" s="19">
+        <v>0.98402777777777783</v>
+      </c>
       <c r="M21" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21" s="19">
+        <v>0.2722222222222222</v>
+      </c>
+      <c r="O21" s="19">
+        <v>0.96319444444444446</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>110</v>
       </c>
@@ -21639,14 +22038,32 @@
       <c r="E22" t="s">
         <v>72</v>
       </c>
+      <c r="F22" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I22" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="J22" t="s">
         <v>242</v>
       </c>
+      <c r="K22" s="19">
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="L22" s="19">
+        <v>0.98263888888888884</v>
+      </c>
       <c r="M22" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22" s="19">
+        <v>0.27430555555555552</v>
+      </c>
+      <c r="O22" s="19">
+        <v>0.96527777777777779</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>111</v>
       </c>
@@ -21662,14 +22079,32 @@
       <c r="E23" t="s">
         <v>72</v>
       </c>
+      <c r="F23" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I23" s="19">
+        <v>0.97569444444444453</v>
+      </c>
       <c r="J23" t="s">
         <v>242</v>
       </c>
+      <c r="K23" s="19">
+        <v>0.2722222222222222</v>
+      </c>
+      <c r="L23" s="19">
+        <v>0.98055555555555562</v>
+      </c>
       <c r="M23" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23" s="19">
+        <v>0.27569444444444446</v>
+      </c>
+      <c r="O23" s="19">
+        <v>0.96666666666666667</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>112</v>
       </c>
@@ -21685,14 +22120,32 @@
       <c r="E24" t="s">
         <v>72</v>
       </c>
+      <c r="F24" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I24" s="19">
+        <v>0.97569444444444453</v>
+      </c>
       <c r="J24" t="s">
         <v>242</v>
       </c>
+      <c r="K24" s="19">
+        <v>0.27430555555555552</v>
+      </c>
+      <c r="L24" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="M24" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24" s="19">
+        <v>0.27152777777777776</v>
+      </c>
+      <c r="O24" s="19">
+        <v>0.96805555555555556</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>113</v>
       </c>
@@ -21708,14 +22161,32 @@
       <c r="E25" t="s">
         <v>72</v>
       </c>
+      <c r="F25" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I25" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="J25" t="s">
         <v>242</v>
       </c>
+      <c r="K25" s="19">
+        <v>0.2722222222222222</v>
+      </c>
+      <c r="L25" s="19">
+        <v>0.97777777777777775</v>
+      </c>
       <c r="M25" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25" s="19">
+        <v>0.2722222222222222</v>
+      </c>
+      <c r="O25" s="19">
+        <v>0.96944444444444444</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>12</v>
       </c>
@@ -21731,14 +22202,32 @@
       <c r="E26" t="s">
         <v>72</v>
       </c>
+      <c r="F26" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I26" s="19">
+        <v>0.97361111111111109</v>
+      </c>
       <c r="J26" t="s">
         <v>242</v>
       </c>
+      <c r="K26" s="19">
+        <v>0.27430555555555552</v>
+      </c>
+      <c r="L26" s="19">
+        <v>0.97638888888888886</v>
+      </c>
       <c r="M26" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26" s="19">
+        <v>0.27152777777777776</v>
+      </c>
+      <c r="O26" s="19">
+        <v>0.97083333333333333</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>114</v>
       </c>
@@ -21754,14 +22243,32 @@
       <c r="E27" t="s">
         <v>72</v>
       </c>
+      <c r="F27" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I27" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="J27" t="s">
         <v>242</v>
       </c>
+      <c r="K27" s="19">
+        <v>0.2722222222222222</v>
+      </c>
+      <c r="L27" s="19">
+        <v>0.97499999999999998</v>
+      </c>
       <c r="M27" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27" s="19">
+        <v>0.2722222222222222</v>
+      </c>
+      <c r="O27" s="19">
+        <v>0.97222222222222221</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>15</v>
       </c>
@@ -21777,14 +22284,32 @@
       <c r="E28" t="s">
         <v>72</v>
       </c>
+      <c r="F28" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I28" s="19">
+        <v>0.97569444444444453</v>
+      </c>
       <c r="J28" t="s">
         <v>242</v>
       </c>
+      <c r="K28" s="19">
+        <v>0.27361111111111108</v>
+      </c>
+      <c r="L28" s="19">
+        <v>0.97361111111111109</v>
+      </c>
       <c r="M28" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28" s="19">
+        <v>0.27152777777777776</v>
+      </c>
+      <c r="O28" s="19">
+        <v>0.97361111111111109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>115</v>
       </c>
@@ -21800,14 +22325,32 @@
       <c r="E29" t="s">
         <v>72</v>
       </c>
+      <c r="F29" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I29" s="19">
+        <v>0.96875</v>
+      </c>
       <c r="J29" t="s">
         <v>242</v>
       </c>
+      <c r="K29" s="19">
+        <v>0.27361111111111108</v>
+      </c>
+      <c r="L29" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="M29" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29" s="19">
+        <v>0.2722222222222222</v>
+      </c>
+      <c r="O29" s="19">
+        <v>0.97430555555555554</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>116</v>
       </c>
@@ -21823,14 +22366,32 @@
       <c r="E30" t="s">
         <v>72</v>
       </c>
+      <c r="F30" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I30" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="J30" t="s">
         <v>242</v>
       </c>
+      <c r="K30" s="19">
+        <v>0.27152777777777776</v>
+      </c>
+      <c r="L30" s="19">
+        <v>0.97152777777777777</v>
+      </c>
       <c r="M30" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30" s="19">
+        <v>0.27361111111111108</v>
+      </c>
+      <c r="O30" s="19">
+        <v>0.97638888888888886</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>35</v>
       </c>
@@ -21846,14 +22407,32 @@
       <c r="E31" t="s">
         <v>72</v>
       </c>
+      <c r="F31" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I31" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="J31" t="s">
         <v>242</v>
       </c>
+      <c r="K31" s="19">
+        <v>0.27430555555555552</v>
+      </c>
+      <c r="L31" s="19">
+        <v>0.96944444444444444</v>
+      </c>
       <c r="M31" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31" s="19">
+        <v>0.27152777777777776</v>
+      </c>
+      <c r="O31" s="19">
+        <v>0.97777777777777775</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>117</v>
       </c>
@@ -21869,14 +22448,32 @@
       <c r="E32" t="s">
         <v>72</v>
       </c>
+      <c r="F32" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I32" s="19">
+        <v>0.97569444444444453</v>
+      </c>
       <c r="J32" t="s">
         <v>242</v>
       </c>
+      <c r="K32" s="19">
+        <v>0.27499999999999997</v>
+      </c>
+      <c r="L32" s="19">
+        <v>0.96805555555555556</v>
+      </c>
       <c r="M32" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32" s="19">
+        <v>0.2722222222222222</v>
+      </c>
+      <c r="O32" s="19">
+        <v>0.97916666666666663</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>106</v>
       </c>
@@ -21892,14 +22489,32 @@
       <c r="E33" t="s">
         <v>72</v>
       </c>
+      <c r="F33" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I33" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="J33" t="s">
         <v>242</v>
       </c>
+      <c r="K33" s="19">
+        <v>0.27152777777777776</v>
+      </c>
+      <c r="L33" s="19">
+        <v>0.96666666666666667</v>
+      </c>
       <c r="M33" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33" s="19">
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="O33" s="19">
+        <v>0.97986111111111107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>118</v>
       </c>
@@ -21915,14 +22530,32 @@
       <c r="E34" t="s">
         <v>72</v>
       </c>
+      <c r="F34" s="21">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I34" s="21">
+        <v>0.97569444444444453</v>
+      </c>
       <c r="J34" t="s">
         <v>242</v>
       </c>
+      <c r="K34" s="21">
+        <v>0.2722222222222222</v>
+      </c>
+      <c r="L34" s="21">
+        <v>0.96597222222222223</v>
+      </c>
       <c r="M34" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34" s="21">
+        <v>0.27430555555555552</v>
+      </c>
+      <c r="O34" s="21">
+        <v>0.98125000000000007</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>119</v>
       </c>
@@ -21938,14 +22571,32 @@
       <c r="E35" t="s">
         <v>72</v>
       </c>
+      <c r="F35" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I35" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="J35" t="s">
         <v>242</v>
       </c>
+      <c r="K35" s="19">
+        <v>0.27361111111111108</v>
+      </c>
+      <c r="L35" s="19">
+        <v>0.96458333333333324</v>
+      </c>
       <c r="M35" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N35" s="19">
+        <v>0.27569444444444446</v>
+      </c>
+      <c r="O35" s="19">
+        <v>0.98263888888888884</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>24</v>
       </c>
@@ -21961,14 +22612,32 @@
       <c r="E36" t="s">
         <v>72</v>
       </c>
+      <c r="F36" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I36" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="J36" t="s">
         <v>242</v>
       </c>
+      <c r="K36" s="19">
+        <v>0.2722222222222222</v>
+      </c>
+      <c r="L36" s="19">
+        <v>0.96319444444444446</v>
+      </c>
       <c r="M36" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N36" s="19">
+        <v>0.27708333333333335</v>
+      </c>
+      <c r="O36" s="19">
+        <v>0.98402777777777783</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>120</v>
       </c>
@@ -21984,14 +22653,32 @@
       <c r="E37" t="s">
         <v>72</v>
       </c>
+      <c r="F37" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I37" s="19">
+        <v>0.98263888888888884</v>
+      </c>
       <c r="J37" t="s">
         <v>242</v>
       </c>
+      <c r="K37" s="19">
+        <v>0.27430555555555552</v>
+      </c>
+      <c r="L37" s="19">
+        <v>0.96180555555555547</v>
+      </c>
       <c r="M37" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="O37" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>108</v>
       </c>
@@ -22007,14 +22694,32 @@
       <c r="E38" t="s">
         <v>71</v>
       </c>
+      <c r="F38" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I38" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="J38" t="s">
         <v>242</v>
       </c>
+      <c r="K38" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="L38" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="M38" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N38" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O38" s="19">
+        <v>0.95138888888888884</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>109</v>
       </c>
@@ -22030,14 +22735,32 @@
       <c r="E39" t="s">
         <v>71</v>
       </c>
+      <c r="F39" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I39" s="19">
+        <v>0.96875</v>
+      </c>
       <c r="J39" t="s">
         <v>242</v>
       </c>
+      <c r="K39" s="19">
+        <v>0.33402777777777781</v>
+      </c>
+      <c r="L39" s="19">
+        <v>0.97361111111111109</v>
+      </c>
       <c r="M39" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N39" s="19">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="O39" s="19">
+        <v>0.95277777777777783</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>110</v>
       </c>
@@ -22053,14 +22776,32 @@
       <c r="E40" t="s">
         <v>71</v>
       </c>
+      <c r="F40" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I40" s="19">
+        <v>0.96875</v>
+      </c>
       <c r="J40" t="s">
         <v>242</v>
       </c>
+      <c r="K40" s="19">
+        <v>0.3354166666666667</v>
+      </c>
+      <c r="L40" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="M40" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N40" s="19">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="O40" s="19">
+        <v>0.95486111111111116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>111</v>
       </c>
@@ -22076,14 +22817,32 @@
       <c r="E41" t="s">
         <v>71</v>
       </c>
+      <c r="F41" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I41" s="19">
+        <v>0.96527777777777779</v>
+      </c>
       <c r="J41" t="s">
         <v>242</v>
       </c>
+      <c r="K41" s="19">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="L41" s="19">
+        <v>0.97013888888888899</v>
+      </c>
       <c r="M41" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N41" s="19">
+        <v>0.33819444444444446</v>
+      </c>
+      <c r="O41" s="19">
+        <v>0.95624999999999993</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>112</v>
       </c>
@@ -22099,14 +22858,32 @@
       <c r="E42" t="s">
         <v>71</v>
       </c>
+      <c r="F42" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I42" s="19">
+        <v>0.96527777777777779</v>
+      </c>
       <c r="J42" t="s">
         <v>242</v>
       </c>
+      <c r="K42" s="19">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="L42" s="19">
+        <v>0.96875</v>
+      </c>
       <c r="M42" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N42" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O42" s="19">
+        <v>0.95763888888888893</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>113</v>
       </c>
@@ -22122,14 +22899,32 @@
       <c r="E43" t="s">
         <v>71</v>
       </c>
+      <c r="F43" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I43" s="19">
+        <v>0.96180555555555547</v>
+      </c>
       <c r="J43" t="s">
         <v>242</v>
       </c>
+      <c r="K43" s="19">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="L43" s="19">
+        <v>0.96736111111111101</v>
+      </c>
       <c r="M43" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N43" s="19">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="O43" s="19">
+        <v>0.9590277777777777</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>12</v>
       </c>
@@ -22145,14 +22940,32 @@
       <c r="E44" t="s">
         <v>71</v>
       </c>
+      <c r="F44" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I44" s="19">
+        <v>0.96180555555555547</v>
+      </c>
       <c r="J44" t="s">
         <v>242</v>
       </c>
+      <c r="K44" s="19">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="L44" s="19">
+        <v>0.96597222222222223</v>
+      </c>
       <c r="M44" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N44" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O44" s="19">
+        <v>0.9604166666666667</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>114</v>
       </c>
@@ -22168,14 +22981,32 @@
       <c r="E45" t="s">
         <v>71</v>
       </c>
+      <c r="F45" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I45" s="19">
+        <v>0.96180555555555547</v>
+      </c>
       <c r="J45" t="s">
         <v>242</v>
       </c>
+      <c r="K45" s="19">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="L45" s="19">
+        <v>0.96458333333333324</v>
+      </c>
       <c r="M45" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N45" s="19">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="O45" s="19">
+        <v>0.96180555555555547</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>15</v>
       </c>
@@ -22191,14 +23022,32 @@
       <c r="E46" t="s">
         <v>71</v>
       </c>
+      <c r="F46" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I46" s="19">
+        <v>0.96250000000000002</v>
+      </c>
       <c r="J46" t="s">
         <v>242</v>
       </c>
+      <c r="K46" s="19">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="L46" s="19">
+        <v>0.96319444444444446</v>
+      </c>
       <c r="M46" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N46" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O46" s="19">
+        <v>0.96319444444444446</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>115</v>
       </c>
@@ -22214,14 +23063,32 @@
       <c r="E47" t="s">
         <v>71</v>
       </c>
+      <c r="F47" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I47" s="19">
+        <v>0.95833333333333337</v>
+      </c>
       <c r="J47" t="s">
         <v>242</v>
       </c>
+      <c r="K47" s="19">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="L47" s="19">
+        <v>0.96180555555555547</v>
+      </c>
       <c r="M47" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N47" s="19">
+        <v>0.33402777777777781</v>
+      </c>
+      <c r="O47" s="19">
+        <v>0.96388888888888891</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>116</v>
       </c>
@@ -22237,14 +23104,32 @@
       <c r="E48" t="s">
         <v>71</v>
       </c>
+      <c r="F48" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I48" s="19">
+        <v>0.96180555555555547</v>
+      </c>
       <c r="J48" t="s">
         <v>242</v>
       </c>
+      <c r="K48" s="19">
+        <v>0.33402777777777781</v>
+      </c>
+      <c r="L48" s="19">
+        <v>0.96111111111111114</v>
+      </c>
       <c r="M48" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N48" s="19">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="O48" s="19">
+        <v>0.96597222222222223</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>35</v>
       </c>
@@ -22260,14 +23145,32 @@
       <c r="E49" t="s">
         <v>71</v>
       </c>
+      <c r="F49" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I49" s="19">
+        <v>0.96180555555555547</v>
+      </c>
       <c r="J49" t="s">
         <v>242</v>
       </c>
+      <c r="K49" s="19">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="L49" s="19">
+        <v>0.9590277777777777</v>
+      </c>
       <c r="M49" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N49" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O49" s="19">
+        <v>0.96736111111111101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>117</v>
       </c>
@@ -22283,14 +23186,32 @@
       <c r="E50" t="s">
         <v>71</v>
       </c>
+      <c r="F50" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I50" s="19">
+        <v>0.96527777777777779</v>
+      </c>
       <c r="J50" t="s">
         <v>242</v>
       </c>
+      <c r="K50" s="19">
+        <v>0.3354166666666667</v>
+      </c>
+      <c r="L50" s="19">
+        <v>0.95763888888888893</v>
+      </c>
       <c r="M50" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N50" s="19">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="O50" s="19">
+        <v>0.96875</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>106</v>
       </c>
@@ -22306,14 +23227,32 @@
       <c r="E51" t="s">
         <v>71</v>
       </c>
+      <c r="F51" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I51" s="19">
+        <v>0.96527777777777779</v>
+      </c>
       <c r="J51" t="s">
         <v>242</v>
       </c>
+      <c r="K51" s="19">
+        <v>0.33402777777777781</v>
+      </c>
+      <c r="L51" s="19">
+        <v>0.95624999999999993</v>
+      </c>
       <c r="M51" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N51" s="19">
+        <v>0.3354166666666667</v>
+      </c>
+      <c r="O51" s="19">
+        <v>0.96944444444444444</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>118</v>
       </c>
@@ -22329,14 +23268,32 @@
       <c r="E52" t="s">
         <v>71</v>
       </c>
+      <c r="F52" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I52" s="19">
+        <v>0.96527777777777779</v>
+      </c>
       <c r="J52" t="s">
         <v>242</v>
       </c>
+      <c r="K52" s="19">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="L52" s="19">
+        <v>0.9555555555555556</v>
+      </c>
       <c r="M52" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N52" s="19">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="O52" s="19">
+        <v>0.97083333333333333</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>119</v>
       </c>
@@ -22352,14 +23309,32 @@
       <c r="E53" t="s">
         <v>71</v>
       </c>
+      <c r="F53" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I53" s="19">
+        <v>0.96875</v>
+      </c>
       <c r="J53" t="s">
         <v>242</v>
       </c>
+      <c r="K53" s="19">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="L53" s="19">
+        <v>0.95416666666666661</v>
+      </c>
       <c r="M53" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N53" s="19">
+        <v>0.33819444444444446</v>
+      </c>
+      <c r="O53" s="19">
+        <v>0.97222222222222221</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>24</v>
       </c>
@@ -22375,14 +23350,32 @@
       <c r="E54" t="s">
         <v>71</v>
       </c>
+      <c r="F54" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I54" s="19">
+        <v>0.96875</v>
+      </c>
       <c r="J54" t="s">
         <v>242</v>
       </c>
+      <c r="K54" s="19">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="L54" s="19">
+        <v>0.95277777777777783</v>
+      </c>
       <c r="M54" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N54" s="19">
+        <v>0.33958333333333335</v>
+      </c>
+      <c r="O54" s="19">
+        <v>0.97361111111111109</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>120</v>
       </c>
@@ -22398,11 +23391,29 @@
       <c r="E55" t="s">
         <v>71</v>
       </c>
+      <c r="F55" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I55" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="J55" t="s">
         <v>242</v>
       </c>
+      <c r="K55" s="19">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="L55" s="19">
+        <v>0.95138888888888884</v>
+      </c>
       <c r="M55" t="s">
         <v>267</v>
+      </c>
+      <c r="N55" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="O55" s="20" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -22414,8 +23425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P409"/>
   <sheetViews>
-    <sheetView topLeftCell="A372" workbookViewId="0">
-      <selection sqref="A1:D409"/>
+    <sheetView tabSelected="1" topLeftCell="A374" workbookViewId="0">
+      <selection sqref="A1:P409"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38462,13 +39473,13 @@
     </row>
     <row r="328" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A328">
-        <v>202</v>
+        <v>103</v>
       </c>
       <c r="B328" t="s">
-        <v>232</v>
+        <v>280</v>
       </c>
       <c r="C328" t="s">
-        <v>231</v>
+        <v>279</v>
       </c>
       <c r="D328" t="s">
         <v>228</v>
@@ -38872,13 +39883,13 @@
     </row>
     <row r="338" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A338">
-        <v>202</v>
+        <v>103</v>
       </c>
       <c r="B338" t="s">
-        <v>232</v>
+        <v>280</v>
       </c>
       <c r="C338" t="s">
-        <v>231</v>
+        <v>279</v>
       </c>
       <c r="D338" t="s">
         <v>228</v>
@@ -39282,13 +40293,13 @@
     </row>
     <row r="348" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A348">
-        <v>202</v>
+        <v>103</v>
       </c>
       <c r="B348" t="s">
-        <v>232</v>
+        <v>280</v>
       </c>
       <c r="C348" t="s">
-        <v>231</v>
+        <v>279</v>
       </c>
       <c r="D348" t="s">
         <v>228</v>
@@ -39608,7 +40619,7 @@
         <v>0.98263888888888884</v>
       </c>
     </row>
-    <row r="356" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A356">
         <v>108</v>
       </c>
@@ -39624,14 +40635,32 @@
       <c r="E356" t="s">
         <v>9</v>
       </c>
+      <c r="F356" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I356" s="19">
+        <v>0.98263888888888884</v>
+      </c>
       <c r="J356" t="s">
         <v>242</v>
       </c>
+      <c r="K356" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="L356" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="M356" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="357" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N356" s="19">
+        <v>0.24374999999999999</v>
+      </c>
+      <c r="O356" s="19">
+        <v>0.96180555555555547</v>
+      </c>
+    </row>
+    <row r="357" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A357">
         <v>109</v>
       </c>
@@ -39647,14 +40676,32 @@
       <c r="E357" t="s">
         <v>9</v>
       </c>
+      <c r="F357" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I357" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="J357" t="s">
         <v>242</v>
       </c>
+      <c r="K357" s="19">
+        <v>0.24374999999999999</v>
+      </c>
+      <c r="L357" s="19">
+        <v>0.98402777777777783</v>
+      </c>
       <c r="M357" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="358" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N357" s="19">
+        <v>0.24444444444444446</v>
+      </c>
+      <c r="O357" s="19">
+        <v>0.96319444444444446</v>
+      </c>
+    </row>
+    <row r="358" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A358">
         <v>110</v>
       </c>
@@ -39670,14 +40717,32 @@
       <c r="E358" t="s">
         <v>9</v>
       </c>
+      <c r="F358" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I358" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="J358" t="s">
         <v>242</v>
       </c>
+      <c r="K358" s="19">
+        <v>0.24513888888888888</v>
+      </c>
+      <c r="L358" s="19">
+        <v>0.98263888888888884</v>
+      </c>
       <c r="M358" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="359" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N358" s="19">
+        <v>0.24652777777777779</v>
+      </c>
+      <c r="O358" s="19">
+        <v>0.96527777777777779</v>
+      </c>
+    </row>
+    <row r="359" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A359">
         <v>111</v>
       </c>
@@ -39693,14 +40758,32 @@
       <c r="E359" t="s">
         <v>9</v>
       </c>
+      <c r="F359" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I359" s="19">
+        <v>0.97569444444444453</v>
+      </c>
       <c r="J359" t="s">
         <v>242</v>
       </c>
+      <c r="K359" s="19">
+        <v>0.24444444444444446</v>
+      </c>
+      <c r="L359" s="19">
+        <v>0.98055555555555562</v>
+      </c>
       <c r="M359" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="360" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N359" s="19">
+        <v>0.24791666666666667</v>
+      </c>
+      <c r="O359" s="19">
+        <v>0.96666666666666667</v>
+      </c>
+    </row>
+    <row r="360" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A360">
         <v>112</v>
       </c>
@@ -39716,14 +40799,32 @@
       <c r="E360" t="s">
         <v>9</v>
       </c>
+      <c r="F360" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I360" s="19">
+        <v>0.97569444444444453</v>
+      </c>
       <c r="J360" t="s">
         <v>242</v>
       </c>
+      <c r="K360" s="19">
+        <v>0.24583333333333335</v>
+      </c>
+      <c r="L360" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="M360" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="361" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N360" s="19">
+        <v>0.24374999999999999</v>
+      </c>
+      <c r="O360" s="19">
+        <v>0.96805555555555556</v>
+      </c>
+    </row>
+    <row r="361" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A361">
         <v>113</v>
       </c>
@@ -39739,14 +40840,32 @@
       <c r="E361" t="s">
         <v>9</v>
       </c>
+      <c r="F361" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I361" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="J361" t="s">
         <v>242</v>
       </c>
+      <c r="K361" s="19">
+        <v>0.24444444444444446</v>
+      </c>
+      <c r="L361" s="19">
+        <v>0.97777777777777775</v>
+      </c>
       <c r="M361" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="362" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N361" s="19">
+        <v>0.24444444444444446</v>
+      </c>
+      <c r="O361" s="19">
+        <v>0.96944444444444444</v>
+      </c>
+    </row>
+    <row r="362" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A362">
         <v>12</v>
       </c>
@@ -39762,14 +40881,32 @@
       <c r="E362" t="s">
         <v>9</v>
       </c>
+      <c r="F362" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I362" s="19">
+        <v>0.97361111111111109</v>
+      </c>
       <c r="J362" t="s">
         <v>242</v>
       </c>
+      <c r="K362" s="19">
+        <v>0.25208333333333333</v>
+      </c>
+      <c r="L362" s="19">
+        <v>0.97638888888888886</v>
+      </c>
       <c r="M362" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="363" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N362" s="19">
+        <v>0.25138888888888888</v>
+      </c>
+      <c r="O362" s="19">
+        <v>0.97083333333333333</v>
+      </c>
+    </row>
+    <row r="363" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A363">
         <v>114</v>
       </c>
@@ -39785,14 +40922,32 @@
       <c r="E363" t="s">
         <v>9</v>
       </c>
+      <c r="F363" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I363" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="J363" t="s">
         <v>242</v>
       </c>
+      <c r="K363" s="19">
+        <v>0.24444444444444446</v>
+      </c>
+      <c r="L363" s="19">
+        <v>0.97499999999999998</v>
+      </c>
       <c r="M363" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="364" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N363" s="19">
+        <v>0.24444444444444446</v>
+      </c>
+      <c r="O363" s="19">
+        <v>0.97222222222222221</v>
+      </c>
+    </row>
+    <row r="364" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A364">
         <v>15</v>
       </c>
@@ -39808,14 +40963,32 @@
       <c r="E364" t="s">
         <v>9</v>
       </c>
+      <c r="F364" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I364" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="J364" t="s">
         <v>242</v>
       </c>
+      <c r="K364" s="19">
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="L364" s="19">
+        <v>0.97361111111111109</v>
+      </c>
       <c r="M364" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="365" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N364" s="19">
+        <v>0.2388888888888889</v>
+      </c>
+      <c r="O364" s="19">
+        <v>0.97361111111111109</v>
+      </c>
+    </row>
+    <row r="365" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A365">
         <v>115</v>
       </c>
@@ -39831,14 +41004,32 @@
       <c r="E365" t="s">
         <v>9</v>
       </c>
+      <c r="F365" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I365" s="19">
+        <v>0.96875</v>
+      </c>
       <c r="J365" t="s">
         <v>242</v>
       </c>
+      <c r="K365" s="19">
+        <v>0.24583333333333335</v>
+      </c>
+      <c r="L365" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="M365" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="366" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N365" s="19">
+        <v>0.24374999999999999</v>
+      </c>
+      <c r="O365" s="19">
+        <v>0.97430555555555554</v>
+      </c>
+    </row>
+    <row r="366" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A366">
         <v>116</v>
       </c>
@@ -39854,14 +41045,32 @@
       <c r="E366" t="s">
         <v>9</v>
       </c>
+      <c r="F366" s="21">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I366" s="21">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="J366" t="s">
         <v>242</v>
       </c>
+      <c r="K366" s="21">
+        <v>0.24374999999999999</v>
+      </c>
+      <c r="L366" s="21">
+        <v>0.97152777777777777</v>
+      </c>
       <c r="M366" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="367" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N366" s="21">
+        <v>0.24583333333333335</v>
+      </c>
+      <c r="O366" s="21">
+        <v>0.97638888888888886</v>
+      </c>
+    </row>
+    <row r="367" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A367">
         <v>35</v>
       </c>
@@ -39877,14 +41086,32 @@
       <c r="E367" t="s">
         <v>9</v>
       </c>
+      <c r="F367" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I367" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="J367" t="s">
         <v>242</v>
       </c>
+      <c r="K367" s="19">
+        <v>0.24583333333333335</v>
+      </c>
+      <c r="L367" s="19">
+        <v>0.96944444444444444</v>
+      </c>
       <c r="M367" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="368" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N367" s="19">
+        <v>0.24374999999999999</v>
+      </c>
+      <c r="O367" s="19">
+        <v>0.97777777777777775</v>
+      </c>
+    </row>
+    <row r="368" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A368">
         <v>117</v>
       </c>
@@ -39900,14 +41127,32 @@
       <c r="E368" t="s">
         <v>9</v>
       </c>
+      <c r="F368" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I368" s="19">
+        <v>0.97569444444444453</v>
+      </c>
       <c r="J368" t="s">
         <v>242</v>
       </c>
+      <c r="K368" s="19">
+        <v>0.24444444444444446</v>
+      </c>
+      <c r="L368" s="19">
+        <v>0.96805555555555556</v>
+      </c>
       <c r="M368" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="369" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N368" s="19">
+        <v>0.24444444444444446</v>
+      </c>
+      <c r="O368" s="19">
+        <v>0.97916666666666663</v>
+      </c>
+    </row>
+    <row r="369" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A369">
         <v>106</v>
       </c>
@@ -39923,14 +41168,32 @@
       <c r="E369" t="s">
         <v>9</v>
       </c>
+      <c r="F369" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I369" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="J369" t="s">
         <v>242</v>
       </c>
+      <c r="K369" s="19">
+        <v>0.23819444444444446</v>
+      </c>
+      <c r="L369" s="19">
+        <v>0.96666666666666667</v>
+      </c>
       <c r="M369" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="370" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N369" s="19">
+        <v>0.23819444444444446</v>
+      </c>
+      <c r="O369" s="19">
+        <v>0.97986111111111107</v>
+      </c>
+    </row>
+    <row r="370" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A370">
         <v>118</v>
       </c>
@@ -39946,14 +41209,32 @@
       <c r="E370" t="s">
         <v>9</v>
       </c>
+      <c r="F370" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I370" s="19">
+        <v>0.97569444444444453</v>
+      </c>
       <c r="J370" t="s">
         <v>242</v>
       </c>
+      <c r="K370" s="19">
+        <v>0.24444444444444446</v>
+      </c>
+      <c r="L370" s="19">
+        <v>0.96597222222222223</v>
+      </c>
       <c r="M370" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="371" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N370" s="19">
+        <v>0.24652777777777779</v>
+      </c>
+      <c r="O370" s="19">
+        <v>0.98125000000000007</v>
+      </c>
+    </row>
+    <row r="371" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A371">
         <v>119</v>
       </c>
@@ -39969,14 +41250,32 @@
       <c r="E371" t="s">
         <v>9</v>
       </c>
+      <c r="F371" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I371" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="J371" t="s">
         <v>242</v>
       </c>
+      <c r="K371" s="19">
+        <v>0.24583333333333335</v>
+      </c>
+      <c r="L371" s="19">
+        <v>0.96458333333333324</v>
+      </c>
       <c r="M371" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="372" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N371" s="19">
+        <v>0.24791666666666667</v>
+      </c>
+      <c r="O371" s="19">
+        <v>0.98263888888888884</v>
+      </c>
+    </row>
+    <row r="372" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A372">
         <v>24</v>
       </c>
@@ -39992,14 +41291,32 @@
       <c r="E372" t="s">
         <v>9</v>
       </c>
+      <c r="F372" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I372" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="J372" t="s">
         <v>242</v>
       </c>
+      <c r="K372" s="19">
+        <v>0.24444444444444446</v>
+      </c>
+      <c r="L372" s="19">
+        <v>0.96319444444444446</v>
+      </c>
       <c r="M372" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="373" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N372" s="19">
+        <v>0.24930555555555556</v>
+      </c>
+      <c r="O372" s="19">
+        <v>0.98402777777777783</v>
+      </c>
+    </row>
+    <row r="373" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A373">
         <v>120</v>
       </c>
@@ -40015,14 +41332,32 @@
       <c r="E373" t="s">
         <v>9</v>
       </c>
+      <c r="F373" s="19">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="I373" s="19">
+        <v>0.98263888888888884</v>
+      </c>
       <c r="J373" t="s">
         <v>242</v>
       </c>
+      <c r="K373" s="19">
+        <v>0.24583333333333335</v>
+      </c>
+      <c r="L373" s="19">
+        <v>0.96180555555555547</v>
+      </c>
       <c r="M373" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="374" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N373" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="O373" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="374" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A374">
         <v>108</v>
       </c>
@@ -40038,14 +41373,32 @@
       <c r="E374" t="s">
         <v>72</v>
       </c>
+      <c r="F374" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I374" s="19">
+        <v>0.98263888888888884</v>
+      </c>
       <c r="J374" t="s">
         <v>242</v>
       </c>
+      <c r="K374" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="L374" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="M374" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="375" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N374" s="19">
+        <v>0.27152777777777776</v>
+      </c>
+      <c r="O374" s="19">
+        <v>0.96180555555555547</v>
+      </c>
+    </row>
+    <row r="375" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A375">
         <v>109</v>
       </c>
@@ -40061,14 +41414,32 @@
       <c r="E375" t="s">
         <v>72</v>
       </c>
+      <c r="F375" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I375" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="J375" t="s">
         <v>242</v>
       </c>
+      <c r="K375" s="19">
+        <v>0.27152777777777776</v>
+      </c>
+      <c r="L375" s="19">
+        <v>0.98402777777777783</v>
+      </c>
       <c r="M375" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="376" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N375" s="19">
+        <v>0.2722222222222222</v>
+      </c>
+      <c r="O375" s="19">
+        <v>0.96319444444444446</v>
+      </c>
+    </row>
+    <row r="376" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A376">
         <v>110</v>
       </c>
@@ -40084,14 +41455,32 @@
       <c r="E376" t="s">
         <v>72</v>
       </c>
+      <c r="F376" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I376" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="J376" t="s">
         <v>242</v>
       </c>
+      <c r="K376" s="19">
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="L376" s="19">
+        <v>0.98263888888888884</v>
+      </c>
       <c r="M376" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="377" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N376" s="19">
+        <v>0.27430555555555552</v>
+      </c>
+      <c r="O376" s="19">
+        <v>0.96527777777777779</v>
+      </c>
+    </row>
+    <row r="377" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A377">
         <v>111</v>
       </c>
@@ -40107,14 +41496,32 @@
       <c r="E377" t="s">
         <v>72</v>
       </c>
+      <c r="F377" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I377" s="19">
+        <v>0.97569444444444453</v>
+      </c>
       <c r="J377" t="s">
         <v>242</v>
       </c>
+      <c r="K377" s="19">
+        <v>0.2722222222222222</v>
+      </c>
+      <c r="L377" s="19">
+        <v>0.98055555555555562</v>
+      </c>
       <c r="M377" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="378" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N377" s="19">
+        <v>0.27569444444444446</v>
+      </c>
+      <c r="O377" s="19">
+        <v>0.96666666666666667</v>
+      </c>
+    </row>
+    <row r="378" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A378">
         <v>112</v>
       </c>
@@ -40130,14 +41537,32 @@
       <c r="E378" t="s">
         <v>72</v>
       </c>
+      <c r="F378" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I378" s="19">
+        <v>0.97569444444444453</v>
+      </c>
       <c r="J378" t="s">
         <v>242</v>
       </c>
+      <c r="K378" s="19">
+        <v>0.27430555555555552</v>
+      </c>
+      <c r="L378" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="M378" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="379" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N378" s="19">
+        <v>0.27152777777777776</v>
+      </c>
+      <c r="O378" s="19">
+        <v>0.96805555555555556</v>
+      </c>
+    </row>
+    <row r="379" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A379">
         <v>113</v>
       </c>
@@ -40153,14 +41578,32 @@
       <c r="E379" t="s">
         <v>72</v>
       </c>
+      <c r="F379" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I379" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="J379" t="s">
         <v>242</v>
       </c>
+      <c r="K379" s="19">
+        <v>0.2722222222222222</v>
+      </c>
+      <c r="L379" s="19">
+        <v>0.97777777777777775</v>
+      </c>
       <c r="M379" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="380" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N379" s="19">
+        <v>0.2722222222222222</v>
+      </c>
+      <c r="O379" s="19">
+        <v>0.96944444444444444</v>
+      </c>
+    </row>
+    <row r="380" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A380">
         <v>12</v>
       </c>
@@ -40176,14 +41619,32 @@
       <c r="E380" t="s">
         <v>72</v>
       </c>
+      <c r="F380" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I380" s="19">
+        <v>0.97361111111111109</v>
+      </c>
       <c r="J380" t="s">
         <v>242</v>
       </c>
+      <c r="K380" s="19">
+        <v>0.27430555555555552</v>
+      </c>
+      <c r="L380" s="19">
+        <v>0.97638888888888886</v>
+      </c>
       <c r="M380" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="381" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N380" s="19">
+        <v>0.27152777777777776</v>
+      </c>
+      <c r="O380" s="19">
+        <v>0.97083333333333333</v>
+      </c>
+    </row>
+    <row r="381" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A381">
         <v>114</v>
       </c>
@@ -40199,14 +41660,32 @@
       <c r="E381" t="s">
         <v>72</v>
       </c>
+      <c r="F381" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I381" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="J381" t="s">
         <v>242</v>
       </c>
+      <c r="K381" s="19">
+        <v>0.2722222222222222</v>
+      </c>
+      <c r="L381" s="19">
+        <v>0.97499999999999998</v>
+      </c>
       <c r="M381" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="382" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N381" s="19">
+        <v>0.2722222222222222</v>
+      </c>
+      <c r="O381" s="19">
+        <v>0.97222222222222221</v>
+      </c>
+    </row>
+    <row r="382" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A382">
         <v>15</v>
       </c>
@@ -40222,14 +41701,32 @@
       <c r="E382" t="s">
         <v>72</v>
       </c>
+      <c r="F382" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I382" s="19">
+        <v>0.97569444444444453</v>
+      </c>
       <c r="J382" t="s">
         <v>242</v>
       </c>
+      <c r="K382" s="19">
+        <v>0.27361111111111108</v>
+      </c>
+      <c r="L382" s="19">
+        <v>0.97361111111111109</v>
+      </c>
       <c r="M382" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="383" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N382" s="19">
+        <v>0.27152777777777776</v>
+      </c>
+      <c r="O382" s="19">
+        <v>0.97361111111111109</v>
+      </c>
+    </row>
+    <row r="383" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A383">
         <v>115</v>
       </c>
@@ -40245,14 +41742,32 @@
       <c r="E383" t="s">
         <v>72</v>
       </c>
+      <c r="F383" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I383" s="19">
+        <v>0.96875</v>
+      </c>
       <c r="J383" t="s">
         <v>242</v>
       </c>
+      <c r="K383" s="19">
+        <v>0.27361111111111108</v>
+      </c>
+      <c r="L383" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="M383" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="384" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N383" s="19">
+        <v>0.2722222222222222</v>
+      </c>
+      <c r="O383" s="19">
+        <v>0.97430555555555554</v>
+      </c>
+    </row>
+    <row r="384" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A384">
         <v>116</v>
       </c>
@@ -40268,14 +41783,32 @@
       <c r="E384" t="s">
         <v>72</v>
       </c>
+      <c r="F384" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I384" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="J384" t="s">
         <v>242</v>
       </c>
+      <c r="K384" s="19">
+        <v>0.27152777777777776</v>
+      </c>
+      <c r="L384" s="19">
+        <v>0.97152777777777777</v>
+      </c>
       <c r="M384" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="385" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N384" s="19">
+        <v>0.27361111111111108</v>
+      </c>
+      <c r="O384" s="19">
+        <v>0.97638888888888886</v>
+      </c>
+    </row>
+    <row r="385" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A385">
         <v>35</v>
       </c>
@@ -40291,14 +41824,32 @@
       <c r="E385" t="s">
         <v>72</v>
       </c>
+      <c r="F385" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I385" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="J385" t="s">
         <v>242</v>
       </c>
+      <c r="K385" s="19">
+        <v>0.27430555555555552</v>
+      </c>
+      <c r="L385" s="19">
+        <v>0.96944444444444444</v>
+      </c>
       <c r="M385" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="386" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N385" s="19">
+        <v>0.27152777777777776</v>
+      </c>
+      <c r="O385" s="19">
+        <v>0.97777777777777775</v>
+      </c>
+    </row>
+    <row r="386" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A386">
         <v>117</v>
       </c>
@@ -40314,14 +41865,32 @@
       <c r="E386" t="s">
         <v>72</v>
       </c>
+      <c r="F386" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I386" s="19">
+        <v>0.97569444444444453</v>
+      </c>
       <c r="J386" t="s">
         <v>242</v>
       </c>
+      <c r="K386" s="19">
+        <v>0.27499999999999997</v>
+      </c>
+      <c r="L386" s="19">
+        <v>0.96805555555555556</v>
+      </c>
       <c r="M386" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="387" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N386" s="19">
+        <v>0.2722222222222222</v>
+      </c>
+      <c r="O386" s="19">
+        <v>0.97916666666666663</v>
+      </c>
+    </row>
+    <row r="387" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A387">
         <v>106</v>
       </c>
@@ -40337,14 +41906,32 @@
       <c r="E387" t="s">
         <v>72</v>
       </c>
+      <c r="F387" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I387" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="J387" t="s">
         <v>242</v>
       </c>
+      <c r="K387" s="19">
+        <v>0.27152777777777776</v>
+      </c>
+      <c r="L387" s="19">
+        <v>0.96666666666666667</v>
+      </c>
       <c r="M387" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="388" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N387" s="19">
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="O387" s="19">
+        <v>0.97986111111111107</v>
+      </c>
+    </row>
+    <row r="388" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A388">
         <v>118</v>
       </c>
@@ -40360,14 +41947,32 @@
       <c r="E388" t="s">
         <v>72</v>
       </c>
+      <c r="F388" s="21">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I388" s="21">
+        <v>0.97569444444444453</v>
+      </c>
       <c r="J388" t="s">
         <v>242</v>
       </c>
+      <c r="K388" s="21">
+        <v>0.2722222222222222</v>
+      </c>
+      <c r="L388" s="21">
+        <v>0.96597222222222223</v>
+      </c>
       <c r="M388" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="389" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N388" s="21">
+        <v>0.27430555555555552</v>
+      </c>
+      <c r="O388" s="21">
+        <v>0.98125000000000007</v>
+      </c>
+    </row>
+    <row r="389" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A389">
         <v>119</v>
       </c>
@@ -40383,14 +41988,32 @@
       <c r="E389" t="s">
         <v>72</v>
       </c>
+      <c r="F389" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I389" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="J389" t="s">
         <v>242</v>
       </c>
+      <c r="K389" s="19">
+        <v>0.27361111111111108</v>
+      </c>
+      <c r="L389" s="19">
+        <v>0.96458333333333324</v>
+      </c>
       <c r="M389" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="390" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N389" s="19">
+        <v>0.27569444444444446</v>
+      </c>
+      <c r="O389" s="19">
+        <v>0.98263888888888884</v>
+      </c>
+    </row>
+    <row r="390" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A390">
         <v>24</v>
       </c>
@@ -40406,14 +42029,32 @@
       <c r="E390" t="s">
         <v>72</v>
       </c>
+      <c r="F390" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I390" s="19">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="J390" t="s">
         <v>242</v>
       </c>
+      <c r="K390" s="19">
+        <v>0.2722222222222222</v>
+      </c>
+      <c r="L390" s="19">
+        <v>0.96319444444444446</v>
+      </c>
       <c r="M390" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="391" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N390" s="19">
+        <v>0.27708333333333335</v>
+      </c>
+      <c r="O390" s="19">
+        <v>0.98402777777777783</v>
+      </c>
+    </row>
+    <row r="391" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A391">
         <v>120</v>
       </c>
@@ -40429,14 +42070,32 @@
       <c r="E391" t="s">
         <v>72</v>
       </c>
+      <c r="F391" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="I391" s="19">
+        <v>0.98263888888888884</v>
+      </c>
       <c r="J391" t="s">
         <v>242</v>
       </c>
+      <c r="K391" s="19">
+        <v>0.27430555555555552</v>
+      </c>
+      <c r="L391" s="19">
+        <v>0.96180555555555547</v>
+      </c>
       <c r="M391" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="392" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N391" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="O391" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="392" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A392">
         <v>108</v>
       </c>
@@ -40452,14 +42111,32 @@
       <c r="E392" t="s">
         <v>71</v>
       </c>
+      <c r="F392" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I392" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="J392" t="s">
         <v>242</v>
       </c>
+      <c r="K392" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="L392" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="M392" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="393" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N392" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O392" s="19">
+        <v>0.95138888888888884</v>
+      </c>
+    </row>
+    <row r="393" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A393">
         <v>109</v>
       </c>
@@ -40475,14 +42152,32 @@
       <c r="E393" t="s">
         <v>71</v>
       </c>
+      <c r="F393" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I393" s="19">
+        <v>0.96875</v>
+      </c>
       <c r="J393" t="s">
         <v>242</v>
       </c>
+      <c r="K393" s="19">
+        <v>0.33402777777777781</v>
+      </c>
+      <c r="L393" s="19">
+        <v>0.97361111111111109</v>
+      </c>
       <c r="M393" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="394" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N393" s="19">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="O393" s="19">
+        <v>0.95277777777777783</v>
+      </c>
+    </row>
+    <row r="394" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A394">
         <v>110</v>
       </c>
@@ -40498,14 +42193,32 @@
       <c r="E394" t="s">
         <v>71</v>
       </c>
+      <c r="F394" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I394" s="19">
+        <v>0.96875</v>
+      </c>
       <c r="J394" t="s">
         <v>242</v>
       </c>
+      <c r="K394" s="19">
+        <v>0.3354166666666667</v>
+      </c>
+      <c r="L394" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="M394" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="395" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N394" s="19">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="O394" s="19">
+        <v>0.95486111111111116</v>
+      </c>
+    </row>
+    <row r="395" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A395">
         <v>111</v>
       </c>
@@ -40521,14 +42234,32 @@
       <c r="E395" t="s">
         <v>71</v>
       </c>
+      <c r="F395" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I395" s="19">
+        <v>0.96527777777777779</v>
+      </c>
       <c r="J395" t="s">
         <v>242</v>
       </c>
+      <c r="K395" s="19">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="L395" s="19">
+        <v>0.97013888888888899</v>
+      </c>
       <c r="M395" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="396" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N395" s="19">
+        <v>0.33819444444444446</v>
+      </c>
+      <c r="O395" s="19">
+        <v>0.95624999999999993</v>
+      </c>
+    </row>
+    <row r="396" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A396">
         <v>112</v>
       </c>
@@ -40544,14 +42275,32 @@
       <c r="E396" t="s">
         <v>71</v>
       </c>
+      <c r="F396" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I396" s="19">
+        <v>0.96527777777777779</v>
+      </c>
       <c r="J396" t="s">
         <v>242</v>
       </c>
+      <c r="K396" s="19">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="L396" s="19">
+        <v>0.96875</v>
+      </c>
       <c r="M396" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="397" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N396" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O396" s="19">
+        <v>0.95763888888888893</v>
+      </c>
+    </row>
+    <row r="397" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A397">
         <v>113</v>
       </c>
@@ -40567,14 +42316,32 @@
       <c r="E397" t="s">
         <v>71</v>
       </c>
+      <c r="F397" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I397" s="19">
+        <v>0.96180555555555547</v>
+      </c>
       <c r="J397" t="s">
         <v>242</v>
       </c>
+      <c r="K397" s="19">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="L397" s="19">
+        <v>0.96736111111111101</v>
+      </c>
       <c r="M397" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="398" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N397" s="19">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="O397" s="19">
+        <v>0.9590277777777777</v>
+      </c>
+    </row>
+    <row r="398" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A398">
         <v>12</v>
       </c>
@@ -40590,14 +42357,32 @@
       <c r="E398" t="s">
         <v>71</v>
       </c>
+      <c r="F398" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I398" s="19">
+        <v>0.96180555555555547</v>
+      </c>
       <c r="J398" t="s">
         <v>242</v>
       </c>
+      <c r="K398" s="19">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="L398" s="19">
+        <v>0.96597222222222223</v>
+      </c>
       <c r="M398" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="399" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N398" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O398" s="19">
+        <v>0.9604166666666667</v>
+      </c>
+    </row>
+    <row r="399" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A399">
         <v>114</v>
       </c>
@@ -40613,14 +42398,32 @@
       <c r="E399" t="s">
         <v>71</v>
       </c>
+      <c r="F399" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I399" s="19">
+        <v>0.96180555555555547</v>
+      </c>
       <c r="J399" t="s">
         <v>242</v>
       </c>
+      <c r="K399" s="19">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="L399" s="19">
+        <v>0.96458333333333324</v>
+      </c>
       <c r="M399" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="400" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N399" s="19">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="O399" s="19">
+        <v>0.96180555555555547</v>
+      </c>
+    </row>
+    <row r="400" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A400">
         <v>15</v>
       </c>
@@ -40636,14 +42439,32 @@
       <c r="E400" t="s">
         <v>71</v>
       </c>
+      <c r="F400" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I400" s="19">
+        <v>0.96250000000000002</v>
+      </c>
       <c r="J400" t="s">
         <v>242</v>
       </c>
+      <c r="K400" s="19">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="L400" s="19">
+        <v>0.96319444444444446</v>
+      </c>
       <c r="M400" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="401" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N400" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O400" s="19">
+        <v>0.96319444444444446</v>
+      </c>
+    </row>
+    <row r="401" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A401">
         <v>115</v>
       </c>
@@ -40659,14 +42480,32 @@
       <c r="E401" t="s">
         <v>71</v>
       </c>
+      <c r="F401" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I401" s="19">
+        <v>0.95833333333333337</v>
+      </c>
       <c r="J401" t="s">
         <v>242</v>
       </c>
+      <c r="K401" s="19">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="L401" s="19">
+        <v>0.96180555555555547</v>
+      </c>
       <c r="M401" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="402" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N401" s="19">
+        <v>0.33402777777777781</v>
+      </c>
+      <c r="O401" s="19">
+        <v>0.96388888888888891</v>
+      </c>
+    </row>
+    <row r="402" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A402">
         <v>116</v>
       </c>
@@ -40682,14 +42521,32 @@
       <c r="E402" t="s">
         <v>71</v>
       </c>
+      <c r="F402" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I402" s="19">
+        <v>0.96180555555555547</v>
+      </c>
       <c r="J402" t="s">
         <v>242</v>
       </c>
+      <c r="K402" s="19">
+        <v>0.33402777777777781</v>
+      </c>
+      <c r="L402" s="19">
+        <v>0.96111111111111114</v>
+      </c>
       <c r="M402" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="403" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N402" s="19">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="O402" s="19">
+        <v>0.96597222222222223</v>
+      </c>
+    </row>
+    <row r="403" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A403">
         <v>35</v>
       </c>
@@ -40705,14 +42562,32 @@
       <c r="E403" t="s">
         <v>71</v>
       </c>
+      <c r="F403" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I403" s="19">
+        <v>0.96180555555555547</v>
+      </c>
       <c r="J403" t="s">
         <v>242</v>
       </c>
+      <c r="K403" s="19">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="L403" s="19">
+        <v>0.9590277777777777</v>
+      </c>
       <c r="M403" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="404" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N403" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O403" s="19">
+        <v>0.96736111111111101</v>
+      </c>
+    </row>
+    <row r="404" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A404">
         <v>117</v>
       </c>
@@ -40728,14 +42603,32 @@
       <c r="E404" t="s">
         <v>71</v>
       </c>
+      <c r="F404" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I404" s="19">
+        <v>0.96527777777777779</v>
+      </c>
       <c r="J404" t="s">
         <v>242</v>
       </c>
+      <c r="K404" s="19">
+        <v>0.3354166666666667</v>
+      </c>
+      <c r="L404" s="19">
+        <v>0.95763888888888893</v>
+      </c>
       <c r="M404" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="405" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N404" s="19">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="O404" s="19">
+        <v>0.96875</v>
+      </c>
+    </row>
+    <row r="405" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A405">
         <v>106</v>
       </c>
@@ -40751,14 +42644,32 @@
       <c r="E405" t="s">
         <v>71</v>
       </c>
+      <c r="F405" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I405" s="19">
+        <v>0.96527777777777779</v>
+      </c>
       <c r="J405" t="s">
         <v>242</v>
       </c>
+      <c r="K405" s="19">
+        <v>0.33402777777777781</v>
+      </c>
+      <c r="L405" s="19">
+        <v>0.95624999999999993</v>
+      </c>
       <c r="M405" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="406" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N405" s="19">
+        <v>0.3354166666666667</v>
+      </c>
+      <c r="O405" s="19">
+        <v>0.96944444444444444</v>
+      </c>
+    </row>
+    <row r="406" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A406">
         <v>118</v>
       </c>
@@ -40774,14 +42685,32 @@
       <c r="E406" t="s">
         <v>71</v>
       </c>
+      <c r="F406" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I406" s="19">
+        <v>0.96527777777777779</v>
+      </c>
       <c r="J406" t="s">
         <v>242</v>
       </c>
+      <c r="K406" s="19">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="L406" s="19">
+        <v>0.9555555555555556</v>
+      </c>
       <c r="M406" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="407" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N406" s="19">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="O406" s="19">
+        <v>0.97083333333333333</v>
+      </c>
+    </row>
+    <row r="407" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A407">
         <v>119</v>
       </c>
@@ -40797,14 +42726,32 @@
       <c r="E407" t="s">
         <v>71</v>
       </c>
+      <c r="F407" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I407" s="19">
+        <v>0.96875</v>
+      </c>
       <c r="J407" t="s">
         <v>242</v>
       </c>
+      <c r="K407" s="19">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="L407" s="19">
+        <v>0.95416666666666661</v>
+      </c>
       <c r="M407" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="408" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N407" s="19">
+        <v>0.33819444444444446</v>
+      </c>
+      <c r="O407" s="19">
+        <v>0.97222222222222221</v>
+      </c>
+    </row>
+    <row r="408" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A408">
         <v>24</v>
       </c>
@@ -40820,14 +42767,32 @@
       <c r="E408" t="s">
         <v>71</v>
       </c>
+      <c r="F408" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I408" s="19">
+        <v>0.96875</v>
+      </c>
       <c r="J408" t="s">
         <v>242</v>
       </c>
+      <c r="K408" s="19">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="L408" s="19">
+        <v>0.95277777777777783</v>
+      </c>
       <c r="M408" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="409" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N408" s="19">
+        <v>0.33958333333333335</v>
+      </c>
+      <c r="O408" s="19">
+        <v>0.97361111111111109</v>
+      </c>
+    </row>
+    <row r="409" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A409">
         <v>120</v>
       </c>
@@ -40843,11 +42808,29 @@
       <c r="E409" t="s">
         <v>71</v>
       </c>
+      <c r="F409" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I409" s="19">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="J409" t="s">
         <v>242</v>
       </c>
+      <c r="K409" s="19">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="L409" s="19">
+        <v>0.95138888888888884</v>
+      </c>
       <c r="M409" t="s">
         <v>267</v>
+      </c>
+      <c r="N409" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="O409" s="20" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -40860,7 +42843,7 @@
   <dimension ref="E1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J2" sqref="J2:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40870,58 +42853,94 @@
   <sheetData>
     <row r="1" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="13"/>
+      <c r="E2" s="20" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="3" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="13"/>
+      <c r="E3" s="20" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="4" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="13"/>
+      <c r="E4" s="20" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="5" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="13"/>
+      <c r="E5" s="20" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="6" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="13"/>
+      <c r="E6" s="20" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="7" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="13"/>
-    </row>
-    <row r="8" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E8" s="13"/>
+      <c r="E7" s="20" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="8" spans="5:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="20" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="9" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E9" s="13"/>
-    </row>
-    <row r="10" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="13"/>
+      <c r="E9" s="20" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="5:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="20" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E11" s="13"/>
+      <c r="E11" s="20" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="12" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="13"/>
+      <c r="E12" s="20" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="13" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E13" s="13"/>
-    </row>
-    <row r="14" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E14" s="13"/>
+      <c r="E13" s="20" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="14" spans="5:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="20" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="15" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E15" s="13"/>
+      <c r="E15" s="20" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="16" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="13"/>
+      <c r="E16" s="20" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="17" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E17" s="13"/>
+      <c r="E17" s="20" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="18" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="13"/>
-    </row>
-    <row r="19" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E19" s="13"/>
+      <c r="E18" s="20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="20" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="20" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E20" s="13"/>

</xml_diff>